<commit_message>
Completed Working with Excel's Solver Tool
</commit_message>
<xml_diff>
--- a/29 - What If Tools/Excel103-AdvancedExercises.xlsx
+++ b/29 - What If Tools/Excel103-AdvancedExercises.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/29 - What If Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="10_ncr:8000_{F5B4C794-7C2C-4A34-A8A1-2394A5AF9022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8455D2E-3D69-4548-B503-9B2A4621D48B}"/>
+  <xr:revisionPtr revIDLastSave="505" documentId="10_ncr:8000_{F5B4C794-7C2C-4A34-A8A1-2394A5AF9022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FAFA902-5DB9-4941-A58E-1C8E8127A896}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="13" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -41,16 +41,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Master Emp List'!$B$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SUMIF Function'!$A$2:$E$272</definedName>
     <definedName name="Monthly_Goal">'IF Function'!$I$2</definedName>
+    <definedName name="solver_adj" localSheetId="17" hidden="1">Solver!$B$5:$E$7</definedName>
     <definedName name="solver_cvg" localSheetId="17" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="17" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="17" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="17" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="17" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="17" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs2" localSheetId="17" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs3" localSheetId="17" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs4" localSheetId="17" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs1" localSheetId="17" hidden="1">Solver!$B$5:$E$5</definedName>
+    <definedName name="solver_lhs2" localSheetId="17" hidden="1">Solver!$B$5:$E$7</definedName>
+    <definedName name="solver_lhs3" localSheetId="17" hidden="1">Solver!$B$6:$E$6</definedName>
+    <definedName name="solver_lhs4" localSheetId="17" hidden="1">Solver!$B$7:$E$7</definedName>
     <definedName name="solver_lhs5" localSheetId="17" hidden="1">Solver!$B$8:$E$8</definedName>
     <definedName name="solver_lhs6" localSheetId="17" hidden="1">Solver!$E$8</definedName>
     <definedName name="solver_lhs7" localSheetId="17" hidden="1">Solver!$E$8</definedName>
@@ -64,24 +65,24 @@
     <definedName name="solver_neg" localSheetId="17" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="17" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="17" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="17" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="17" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'IF Function'!$I$2</definedName>
     <definedName name="solver_opt" localSheetId="17" hidden="1">Solver!$H$8</definedName>
     <definedName name="solver_pre" localSheetId="17" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="17" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="17" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="17" hidden="1">2</definedName>
-    <definedName name="solver_rel3" localSheetId="17" hidden="1">2</definedName>
-    <definedName name="solver_rel4" localSheetId="17" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="17" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="17" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="17" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="17" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="17" hidden="1">2</definedName>
     <definedName name="solver_rel6" localSheetId="17" hidden="1">2</definedName>
     <definedName name="solver_rel7" localSheetId="17" hidden="1">2</definedName>
     <definedName name="solver_rel8" localSheetId="17" hidden="1">2</definedName>
-    <definedName name="solver_rhs1" localSheetId="17" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs2" localSheetId="17" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs3" localSheetId="17" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs4" localSheetId="17" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs1" localSheetId="17" hidden="1">92</definedName>
+    <definedName name="solver_rhs2" localSheetId="17" hidden="1">20</definedName>
+    <definedName name="solver_rhs3" localSheetId="17" hidden="1">45</definedName>
+    <definedName name="solver_rhs4" localSheetId="17" hidden="1">55</definedName>
     <definedName name="solver_rhs5" localSheetId="17" hidden="1">Solver!$B$10:$E$10</definedName>
     <definedName name="solver_rhs6" localSheetId="17" hidden="1">Solver!$E$10</definedName>
     <definedName name="solver_rhs7" localSheetId="17" hidden="1">Solver!$E$10</definedName>
@@ -1968,13 +1969,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4903,10 +4904,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="132"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -4915,11 +4916,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="130" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -4928,11 +4929,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131" t="str">
+      <c r="E4" s="130" t="str">
         <f>CONCATENATE(C4," ",B4)</f>
         <v>Joe Gonzales</v>
       </c>
-      <c r="F4" s="132"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -4941,11 +4942,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131" t="str">
+      <c r="E5" s="130" t="str">
         <f t="shared" ref="E5:E18" si="0">CONCATENATE(C5," ",B5)</f>
         <v>Gail Scote</v>
       </c>
-      <c r="F5" s="132"/>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -4954,11 +4955,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131" t="str">
+      <c r="E6" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Sheryl Kane</v>
       </c>
-      <c r="F6" s="132"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -4967,11 +4968,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131" t="str">
+      <c r="E7" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Kendrick Hapsbuch</v>
       </c>
-      <c r="F7" s="132"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -4980,11 +4981,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131" t="str">
+      <c r="E8" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Mark Henders</v>
       </c>
-      <c r="F8" s="132"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -4993,11 +4994,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131" t="str">
+      <c r="E9" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Katie Atherton</v>
       </c>
-      <c r="F9" s="132"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -5006,11 +5007,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131" t="str">
+      <c r="E10" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Frank Bellwood</v>
       </c>
-      <c r="F10" s="132"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -5019,11 +5020,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131" t="str">
+      <c r="E11" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Linda Cooper</v>
       </c>
-      <c r="F11" s="132"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -5032,11 +5033,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131" t="str">
+      <c r="E12" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Brent Cronwith</v>
       </c>
-      <c r="F12" s="132"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -5045,11 +5046,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131" t="str">
+      <c r="E13" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Sandrae Simpson</v>
       </c>
-      <c r="F13" s="132"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -5058,11 +5059,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131" t="str">
+      <c r="E14" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Randy Sindole</v>
       </c>
-      <c r="F14" s="132"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -5071,11 +5072,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131" t="str">
+      <c r="E15" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Ellen Smith</v>
       </c>
-      <c r="F15" s="132"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -5084,11 +5085,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131" t="str">
+      <c r="E16" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Tuome Vuanuo</v>
       </c>
-      <c r="F16" s="132"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -5097,11 +5098,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131" t="str">
+      <c r="E17" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Tadeuz Szcznyck</v>
       </c>
-      <c r="F17" s="132"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -5110,21 +5111,14 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131" t="str">
+      <c r="E18" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Tammy Wu</v>
       </c>
-      <c r="F18" s="132"/>
+      <c r="F18" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -5135,6 +5129,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5724,8 +5725,8 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -5781,8 +5782,8 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -5845,16 +5846,16 @@
         <v>271</v>
       </c>
       <c r="B5" s="85">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="C5" s="85">
-        <v>1</v>
+        <v>39.999999999999993</v>
       </c>
       <c r="D5" s="85">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="E5" s="85">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="F5" s="73"/>
       <c r="G5" s="84">
@@ -5862,7 +5863,7 @@
       </c>
       <c r="H5" s="83">
         <f>G5*(B5+C5+D5+E5)</f>
-        <v>5</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.5">
@@ -5870,16 +5871,16 @@
         <v>270</v>
       </c>
       <c r="B6" s="87">
-        <v>0</v>
+        <v>32.999999999999986</v>
       </c>
       <c r="C6" s="85">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D6" s="85">
-        <v>0</v>
+        <v>43.000000000000007</v>
       </c>
       <c r="E6" s="85">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F6" s="73"/>
       <c r="G6" s="84">
@@ -5887,7 +5888,7 @@
       </c>
       <c r="H6" s="83">
         <f>G6*(B6+C6+D6+E6)</f>
-        <v>0</v>
+        <v>213.44</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.5">
@@ -5895,16 +5896,16 @@
         <v>269</v>
       </c>
       <c r="B7" s="85">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C7" s="85">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D7" s="85">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="E7" s="85">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="F7" s="73"/>
       <c r="G7" s="84">
@@ -5912,7 +5913,7 @@
       </c>
       <c r="H7" s="83">
         <f>G7*(B7+C7+D7+E7)</f>
-        <v>0</v>
+        <v>258.09999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.5">
@@ -5921,25 +5922,25 @@
       </c>
       <c r="B8" s="82">
         <f>SUM(B5:B7)</f>
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="C8" s="82">
         <f>SUM(C5:C7)</f>
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="D8" s="82">
         <f>SUM(D5:D7)</f>
-        <v>1</v>
+        <v>190</v>
       </c>
       <c r="E8" s="82">
         <f>SUM(E5:E7)</f>
-        <v>1</v>
+        <v>160</v>
       </c>
       <c r="F8" s="73"/>
       <c r="G8" s="81"/>
       <c r="H8" s="104">
         <f>H5+H6+H7</f>
-        <v>5</v>
+        <v>866.54</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="4.5" customHeight="1">

</xml_diff>

<commit_message>
Completed Building Effective Data Tables in Excel
</commit_message>
<xml_diff>
--- a/29 - What If Tools/Excel103-AdvancedExercises.xlsx
+++ b/29 - What If Tools/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/29 - What If Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="505" documentId="10_ncr:8000_{F5B4C794-7C2C-4A34-A8A1-2394A5AF9022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FAFA902-5DB9-4941-A58E-1C8E8127A896}"/>
+  <xr:revisionPtr revIDLastSave="506" documentId="10_ncr:8000_{F5B4C794-7C2C-4A34-A8A1-2394A5AF9022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{830DC1F8-52B7-4D78-98AB-48DEB108837E}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1969,13 +1969,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4904,10 +4904,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="130"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -4916,11 +4916,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -4929,11 +4929,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130" t="str">
+      <c r="E4" s="131" t="str">
         <f>CONCATENATE(C4," ",B4)</f>
         <v>Joe Gonzales</v>
       </c>
-      <c r="F4" s="131"/>
+      <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -4942,11 +4942,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130" t="str">
+      <c r="E5" s="131" t="str">
         <f t="shared" ref="E5:E18" si="0">CONCATENATE(C5," ",B5)</f>
         <v>Gail Scote</v>
       </c>
-      <c r="F5" s="131"/>
+      <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -4955,11 +4955,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130" t="str">
+      <c r="E6" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Sheryl Kane</v>
       </c>
-      <c r="F6" s="131"/>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -4968,11 +4968,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130" t="str">
+      <c r="E7" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Kendrick Hapsbuch</v>
       </c>
-      <c r="F7" s="131"/>
+      <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -4981,11 +4981,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130" t="str">
+      <c r="E8" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Mark Henders</v>
       </c>
-      <c r="F8" s="131"/>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -4994,11 +4994,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130" t="str">
+      <c r="E9" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Katie Atherton</v>
       </c>
-      <c r="F9" s="131"/>
+      <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -5007,11 +5007,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130" t="str">
+      <c r="E10" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Frank Bellwood</v>
       </c>
-      <c r="F10" s="131"/>
+      <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -5020,11 +5020,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130" t="str">
+      <c r="E11" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Linda Cooper</v>
       </c>
-      <c r="F11" s="131"/>
+      <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -5033,11 +5033,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130" t="str">
+      <c r="E12" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Brent Cronwith</v>
       </c>
-      <c r="F12" s="131"/>
+      <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -5046,11 +5046,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130" t="str">
+      <c r="E13" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Sandrae Simpson</v>
       </c>
-      <c r="F13" s="131"/>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -5059,11 +5059,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130" t="str">
+      <c r="E14" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Randy Sindole</v>
       </c>
-      <c r="F14" s="131"/>
+      <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -5072,11 +5072,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130" t="str">
+      <c r="E15" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Ellen Smith</v>
       </c>
-      <c r="F15" s="131"/>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -5085,11 +5085,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130" t="str">
+      <c r="E16" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Tuome Vuanuo</v>
       </c>
-      <c r="F16" s="131"/>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -5098,11 +5098,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130" t="str">
+      <c r="E17" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Tadeuz Szcznyck</v>
       </c>
-      <c r="F17" s="131"/>
+      <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -5111,14 +5111,21 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130" t="str">
+      <c r="E18" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Tammy Wu</v>
       </c>
-      <c r="F18" s="131"/>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -5129,13 +5136,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5782,8 +5782,8 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -5990,8 +5990,8 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -6043,43 +6043,58 @@
       <c r="B8" s="74">
         <v>7.2499999999999995E-2</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12">
+        <f t="dataTable" ref="C8:C14" dt2D="0" dtr="0" r1="C3"/>
+        <v>1590.1751010137643</v>
+      </c>
     </row>
     <row r="9" spans="2:3" ht="15.5">
       <c r="B9" s="74">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12">
+        <v>1625.7805911544106</v>
+      </c>
     </row>
     <row r="10" spans="2:3" ht="15.5">
       <c r="B10" s="74">
         <v>7.7499999999999999E-2</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="12">
+        <v>1661.7232770342728</v>
+      </c>
     </row>
     <row r="11" spans="2:3" ht="15.5">
       <c r="B11" s="74">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="12">
+        <v>1734.5902963096128</v>
+      </c>
     </row>
     <row r="12" spans="2:3" ht="15.5">
       <c r="B12" s="74">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="12">
+        <v>1771.4995836166886</v>
+      </c>
     </row>
     <row r="13" spans="2:3" ht="15.5">
       <c r="B13" s="74">
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="12">
+        <v>1808.7159994580018</v>
+      </c>
     </row>
     <row r="14" spans="2:3" ht="15.5">
       <c r="B14" s="74">
         <v>0.09</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="12">
+        <v>1846.2319999966555</v>
+      </c>
     </row>
   </sheetData>
   <printOptions gridLines="1" gridLinesSet="0"/>

</xml_diff>

<commit_message>
Completed Creating Scenarios in Excel
</commit_message>
<xml_diff>
--- a/29 - What If Tools/Excel103-AdvancedExercises.xlsx
+++ b/29 - What If Tools/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/29 - What If Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="506" documentId="10_ncr:8000_{F5B4C794-7C2C-4A34-A8A1-2394A5AF9022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{830DC1F8-52B7-4D78-98AB-48DEB108837E}"/>
+  <xr:revisionPtr revIDLastSave="507" documentId="10_ncr:8000_{F5B4C794-7C2C-4A34-A8A1-2394A5AF9022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCFB8626-60E2-43A3-B6AE-3912AF226483}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1969,13 +1969,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4904,10 +4904,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="132"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -4916,11 +4916,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="130" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -4929,11 +4929,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131" t="str">
+      <c r="E4" s="130" t="str">
         <f>CONCATENATE(C4," ",B4)</f>
         <v>Joe Gonzales</v>
       </c>
-      <c r="F4" s="132"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -4942,11 +4942,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131" t="str">
+      <c r="E5" s="130" t="str">
         <f t="shared" ref="E5:E18" si="0">CONCATENATE(C5," ",B5)</f>
         <v>Gail Scote</v>
       </c>
-      <c r="F5" s="132"/>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -4955,11 +4955,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131" t="str">
+      <c r="E6" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Sheryl Kane</v>
       </c>
-      <c r="F6" s="132"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -4968,11 +4968,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131" t="str">
+      <c r="E7" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Kendrick Hapsbuch</v>
       </c>
-      <c r="F7" s="132"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -4981,11 +4981,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131" t="str">
+      <c r="E8" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Mark Henders</v>
       </c>
-      <c r="F8" s="132"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -4994,11 +4994,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131" t="str">
+      <c r="E9" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Katie Atherton</v>
       </c>
-      <c r="F9" s="132"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -5007,11 +5007,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131" t="str">
+      <c r="E10" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Frank Bellwood</v>
       </c>
-      <c r="F10" s="132"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -5020,11 +5020,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131" t="str">
+      <c r="E11" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Linda Cooper</v>
       </c>
-      <c r="F11" s="132"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -5033,11 +5033,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131" t="str">
+      <c r="E12" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Brent Cronwith</v>
       </c>
-      <c r="F12" s="132"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -5046,11 +5046,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131" t="str">
+      <c r="E13" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Sandrae Simpson</v>
       </c>
-      <c r="F13" s="132"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -5059,11 +5059,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131" t="str">
+      <c r="E14" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Randy Sindole</v>
       </c>
-      <c r="F14" s="132"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -5072,11 +5072,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131" t="str">
+      <c r="E15" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Ellen Smith</v>
       </c>
-      <c r="F15" s="132"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -5085,11 +5085,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131" t="str">
+      <c r="E16" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Tuome Vuanuo</v>
       </c>
-      <c r="F16" s="132"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -5098,11 +5098,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131" t="str">
+      <c r="E17" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Tadeuz Szcznyck</v>
       </c>
-      <c r="F17" s="132"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -5111,21 +5111,14 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131" t="str">
+      <c r="E18" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Tammy Wu</v>
       </c>
-      <c r="F18" s="132"/>
+      <c r="F18" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -5136,6 +5129,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5990,7 +5990,7 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -11059,7 +11059,7 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C11" sqref="C11:C14"/>
     </sheetView>
   </sheetViews>
@@ -11252,6 +11252,26 @@
       </c>
     </row>
   </sheetData>
+  <scenarios current="0" show="0">
+    <scenario name="Default Scenario" locked="1" count="4" user="james cox" comment="Created by james cox on 03/05/2024">
+      <inputCells r="C11" val="0.033" numFmtId="10"/>
+      <inputCells r="C12" val="0.023" numFmtId="10"/>
+      <inputCells r="C13" val="0.043" numFmtId="10"/>
+      <inputCells r="C14" val="0.011" numFmtId="10"/>
+    </scenario>
+    <scenario name="Best Case Scenario" locked="1" count="4" user="james cox" comment="Created by james cox on 03/05/2024">
+      <inputCells r="C11" val="0.05" numFmtId="10"/>
+      <inputCells r="C12" val="0.08" numFmtId="10"/>
+      <inputCells r="C13" val="0.065" numFmtId="10"/>
+      <inputCells r="C14" val="0.03" numFmtId="10"/>
+    </scenario>
+    <scenario name="Worst Case Scenario" locked="1" count="4" user="james cox" comment="Created by james cox on 03/05/2024">
+      <inputCells r="C11" val="0.01" numFmtId="10"/>
+      <inputCells r="C12" val="0.01" numFmtId="10"/>
+      <inputCells r="C13" val="0.01" numFmtId="10"/>
+      <inputCells r="C14" val="0.01" numFmtId="10"/>
+    </scenario>
+  </scenarios>
   <mergeCells count="1">
     <mergeCell ref="B10:C10"/>
   </mergeCells>

</xml_diff>